<commit_message>
Fixed Variable Name of Income Since it had Extra Spaces
</commit_message>
<xml_diff>
--- a/data_science_2/marketing_campaigns_2/1688639964_datadictionaryresponsetomarketingcampaigns.xlsx
+++ b/data_science_2/marketing_campaigns_2/1688639964_datadictionaryresponsetomarketingcampaigns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrespadilla/Desktop/Education/Materials for School/Caltech AIML Bootcamp/git.repos/CB-AIML-2024/data_science_2/marketing_campaigns_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C619A4DC-36CC-ED4C-991C-194A49B04FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9950210A-138A-7543-874C-D7CFEFA90DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E5883398-D96C-6441-ACBF-F847349789D9}"/>
+    <workbookView xWindow="-14940" yWindow="0" windowWidth="14940" windowHeight="21600" xr2:uid="{E5883398-D96C-6441-ACBF-F847349789D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -182,9 +182,6 @@
     <t>Marital_Status</t>
   </si>
   <si>
-    <t xml:space="preserve"> Income </t>
-  </si>
-  <si>
     <t>Dt_Customer</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>Customer's location</t>
+  </si>
+  <si>
+    <t>Income</t>
   </si>
 </sst>
 </file>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7323FEEA-5F11-5346-A3CB-5B717B5421FC}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,7 +595,7 @@
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -603,7 +603,7 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -611,7 +611,7 @@
         <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -619,15 +619,15 @@
         <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -648,10 +648,10 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -808,10 +808,10 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>